<commit_message>
Added state management using Bloc
</commit_message>
<xml_diff>
--- a/Flutter Projects/real_estate_app/DTT-Assessment-Hour-Log.xlsx
+++ b/Flutter Projects/real_estate_app/DTT-Assessment-Hour-Log.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27804"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27813"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amberwessels/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D61EF8A0-6A22-46EC-B5D8-8A1DF1FEB252}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C316625B-D0E3-4BFD-9D2D-0967CD080FFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2060" yWindow="500" windowWidth="34620" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="43">
   <si>
     <r>
       <rPr>
@@ -172,6 +172,29 @@
     <t>Added 3D model floor plan.</t>
   </si>
   <si>
+    <t>Feedback: UI</t>
+  </si>
+  <si>
+    <t>Added seamless faded scrolling to listview.
+Added close icon to searchbar.
+Fixed maps app not opening when marker is clicked.</t>
+  </si>
+  <si>
+    <t>Feedback: Logic</t>
+  </si>
+  <si>
+    <t>Researched state management using Bloc.</t>
+  </si>
+  <si>
+    <t>Created BottomNavigationBar Cubit and implemented it.</t>
+  </si>
+  <si>
+    <t>Created and implemented  House cubit.</t>
+  </si>
+  <si>
+    <t>Created and implemented Filter cubit.</t>
+  </si>
+  <si>
     <t>Total amount of hours</t>
   </si>
 </sst>
@@ -182,7 +205,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
   </numFmts>
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -252,6 +275,12 @@
       <color indexed="8"/>
       <name val="Open Sans"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Open Sans"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -468,7 +497,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -507,6 +536,9 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1777,10 +1809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6.5" defaultRowHeight="15" customHeight="1"/>
@@ -1794,22 +1826,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="73.5" customHeight="1">
-      <c r="A1" s="21"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
+      <c r="A1" s="22"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
       <c r="E1" s="10"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" ht="46.5" customHeight="1">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="24"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25"/>
     </row>
     <row r="3" spans="1:6" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="16" t="s">
@@ -2139,66 +2171,130 @@
       </c>
       <c r="F22" s="4"/>
     </row>
-    <row r="23" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A23" s="5"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="15"/>
+    <row r="23" spans="1:6" ht="33.75" customHeight="1">
+      <c r="A23" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="17">
+        <v>2</v>
+      </c>
+      <c r="C23" s="18">
+        <v>45461</v>
+      </c>
+      <c r="D23" s="20" t="s">
+        <v>36</v>
+      </c>
       <c r="E23" s="19"/>
       <c r="F23" s="4"/>
     </row>
-    <row r="24" spans="1:6" ht="17.100000000000001" customHeight="1">
-      <c r="A24" s="5"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="15"/>
+    <row r="24" spans="1:6" ht="27.75" customHeight="1">
+      <c r="A24" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B24" s="17">
+        <v>2</v>
+      </c>
+      <c r="C24" s="18">
+        <v>45462</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>38</v>
+      </c>
       <c r="E24" s="19"/>
       <c r="F24" s="4"/>
     </row>
-    <row r="25" spans="1:6" ht="16.350000000000001" customHeight="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-      <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="3"/>
+    <row r="25" spans="1:6" ht="27.75" customHeight="1">
+      <c r="A25" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="17">
+        <v>1</v>
+      </c>
+      <c r="C25" s="18">
+        <v>45462</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" s="19"/>
       <c r="F25" s="4"/>
     </row>
-    <row r="26" spans="1:6" ht="16.350000000000001" customHeight="1">
-      <c r="A26" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="B26" s="14">
-        <f>SUMIF(E4:E24,"&lt;&gt;x",B4:B24)</f>
-        <v>22</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+    <row r="26" spans="1:6" ht="17.100000000000001" customHeight="1">
+      <c r="A26" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="17">
+        <v>3</v>
+      </c>
+      <c r="C26" s="18">
+        <v>45463</v>
+      </c>
+      <c r="D26" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="19"/>
       <c r="F26" s="4"/>
     </row>
-    <row r="27" spans="1:6" ht="16.350000000000001" customHeight="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
+    <row r="27" spans="1:6" ht="17.100000000000001" customHeight="1">
+      <c r="A27" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="17">
+        <v>1</v>
+      </c>
+      <c r="C27" s="18">
+        <v>45463</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" s="19"/>
       <c r="F27" s="4"/>
     </row>
     <row r="28" spans="1:6" ht="16.350000000000001" customHeight="1">
-      <c r="A28" s="6"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
+      <c r="A28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
       <c r="E28" s="3"/>
       <c r="F28" s="4"/>
     </row>
     <row r="29" spans="1:6" ht="16.350000000000001" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="9"/>
+      <c r="A29" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B29" s="14">
+        <f>SUMIF(E4:E27,"&lt;&gt;x",B4:B27)</f>
+        <v>31</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="1:6" ht="16.350000000000001" customHeight="1">
+      <c r="A30" s="6"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="1:6" ht="16.350000000000001" customHeight="1">
+      <c r="A31" s="6"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="1:6" ht="16.350000000000001" customHeight="1">
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>